<commit_message>
name change, added statuses colors, gui resise upd
</commit_message>
<xml_diff>
--- a/Protocols/HeadingDiscrimination_test.xlsx
+++ b/Protocols/HeadingDiscrimination_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>name</t>
   </si>
@@ -236,10 +236,19 @@
     <t>value</t>
   </si>
   <si>
-    <t>increment</t>
-  </si>
-  <si>
     <t>1=vestibular only, 2=visual only, 3=combine , 4=delta+ for Visual , 5=delta+ for Vestibular , 10/12=visual in the dark , 11/13=combined in the dark , 14=delta+ for visual in the dark , 15=delta+ for vistibular in the dark.</t>
+  </si>
+  <si>
+    <t>step_plus</t>
+  </si>
+  <si>
+    <t>step_mult</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>varied</t>
   </si>
 </sst>
 </file>
@@ -558,17 +567,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" customWidth="1"/>
     <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.375" customWidth="1"/>
     <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
@@ -577,7 +586,7 @@
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,24 +612,27 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -635,15 +647,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>74</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -664,15 +676,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>73</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -693,15 +705,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>73</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -722,18 +734,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>73</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -751,15 +763,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>73</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -780,15 +792,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>73</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -809,15 +821,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>73</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -838,15 +850,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>73</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -867,15 +879,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>73</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -896,15 +908,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12">
-        <v>1</v>
+      <c r="C12" t="s">
+        <v>73</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -925,15 +937,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>73</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -954,15 +966,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>73</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -983,15 +995,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>73</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1012,15 +1024,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>73</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1048,8 +1060,8 @@
       <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="C17">
-        <v>1</v>
+      <c r="C17" t="s">
+        <v>73</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1077,8 +1089,8 @@
       <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>73</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1280,8 +1292,8 @@
       <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C25">
-        <v>1</v>
+      <c r="C25" t="s">
+        <v>73</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1309,8 +1321,8 @@
       <c r="B26" t="s">
         <v>65</v>
       </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>73</v>
       </c>
       <c r="D26">
         <v>0</v>

</xml_diff>

<commit_message>
Empty template for connections, moog full cpp code, statuses to global
</commit_message>
<xml_diff>
--- a/Protocols/HeadingDiscrimination_test.xlsx
+++ b/Protocols/HeadingDiscrimination_test.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>nice_name</t>
-  </si>
-  <si>
     <t>editable</t>
   </si>
   <si>
@@ -44,189 +41,90 @@
     <t>STIMULUS_TYPE</t>
   </si>
   <si>
-    <t>Stimulus Type</t>
-  </si>
-  <si>
     <t>HEADING_DIRECTION</t>
   </si>
   <si>
-    <t>Heading Direction</t>
-  </si>
-  <si>
     <t>Amplitudes of discrimination about dicretion plane</t>
   </si>
   <si>
-    <t>DIST</t>
-  </si>
-  <si>
-    <t>Distance</t>
-  </si>
-  <si>
     <t>Distance traveled by the base (cm), OpenGL Distance</t>
   </si>
   <si>
-    <t>STIMULUS_DURATION</t>
-  </si>
-  <si>
-    <t>Stimulus Duration</t>
-  </si>
-  <si>
-    <t>The time the movements takes.</t>
-  </si>
-  <si>
     <t>SIGMA</t>
   </si>
   <si>
-    <t>Sigma</t>
-  </si>
-  <si>
     <t>Number of Sigmas in the Gaussian, OpenGL Number of Gaussians</t>
   </si>
   <si>
     <t>DELTA</t>
   </si>
   <si>
-    <t>Delta</t>
-  </si>
-  <si>
     <t>The delta heading between stimulses vestibular and visual.</t>
   </si>
   <si>
     <t>DISC_PLANE_AZIMUTH</t>
   </si>
   <si>
-    <t>Ref - Azimuth</t>
-  </si>
-  <si>
     <t>Azimuth value of discrimination plane, 0 degrees points to the right</t>
   </si>
   <si>
     <t>DISC_PLANE_ELEVATION</t>
   </si>
   <si>
-    <t>Ref - Elevation</t>
-  </si>
-  <si>
     <t>Discrimination Elevation plane, 0 degrees is level</t>
   </si>
   <si>
     <t>DISC_PLANE_TILT</t>
   </si>
   <si>
-    <t>Ref - Tilt</t>
-  </si>
-  <si>
     <t>Discrimination Tilt plane, 0 degrees is along the AZ plane</t>
   </si>
   <si>
     <t>PRE_TRIAL_TIME</t>
   </si>
   <si>
-    <t>Pre trial time</t>
-  </si>
-  <si>
     <t>The time from the trial begin and start beep occurs.</t>
   </si>
   <si>
     <t>TIMEOUT_TIME</t>
   </si>
   <si>
-    <t>Timeout time</t>
-  </si>
-  <si>
     <t>The time the rat have to press the start buttom , otherwise skipping the trial.</t>
   </si>
   <si>
     <t>START_DELAY</t>
   </si>
   <si>
-    <t>Start Delay</t>
-  </si>
-  <si>
     <t>Delay time between rat in center and trial start.</t>
   </si>
   <si>
     <t>RESPONSE_TIME</t>
   </si>
   <si>
-    <t>Response Time</t>
-  </si>
-  <si>
     <t>The reponse time the rat have to determine left or right after the reward.</t>
   </si>
   <si>
     <t>POST_TRIAL_TIME</t>
   </si>
   <si>
-    <t>Post Trial Time</t>
-  </si>
-  <si>
     <t>The time between the end of the previous trial and the next trial.</t>
   </si>
   <si>
-    <t>RR_HEADINGS</t>
-  </si>
-  <si>
-    <t>RR Headings</t>
-  </si>
-  <si>
-    <t>The randon reward absolute heading size.</t>
-  </si>
-  <si>
-    <t>RR_PROBABILITY</t>
-  </si>
-  <si>
-    <t>RR Probability</t>
-  </si>
-  <si>
-    <t>The probability for right reward in the RR heading directions region.</t>
-  </si>
-  <si>
     <t>ADAPTATION_ANGLE</t>
   </si>
   <si>
-    <t>Adaptation angle</t>
-  </si>
-  <si>
     <t>Specifies adaptation angle to be used in combine stimulus</t>
   </si>
   <si>
-    <t>FIXATION_ONLY</t>
-  </si>
-  <si>
-    <t>ERROR_SOUND</t>
-  </si>
-  <si>
-    <t>CORRECT_CUE_SOUND</t>
-  </si>
-  <si>
-    <t>GO_CUE_SOUND</t>
-  </si>
-  <si>
-    <t>BOTH_SIDE_CUE_SOUND</t>
-  </si>
-  <si>
-    <t>RIGHT_LEFT_PARAMETERS_EQUALS</t>
-  </si>
-  <si>
     <t>COHERENCE_LEFT_STRIP</t>
   </si>
   <si>
-    <t>Coherence Left Strip</t>
-  </si>
-  <si>
     <t>The percentage indicates the probabilty to stay turned on in each frame</t>
   </si>
   <si>
     <t>COHERENCE_RIGHT_STRIP</t>
   </si>
   <si>
-    <t>Coherence Right Strip</t>
-  </si>
-  <si>
-    <t>RR_DELTA</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -236,9 +134,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>1=vestibular only, 2=visual only, 3=combine , 4=delta+ for Visual , 5=delta+ for Vestibular , 10/12=visual in the dark , 11/13=combined in the dark , 14=delta+ for visual in the dark , 15=delta+ for vistibular in the dark.</t>
-  </si>
-  <si>
     <t>step_plus</t>
   </si>
   <si>
@@ -249,6 +144,63 @@
   </si>
   <si>
     <t>varied</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>centimeters (cm)</t>
+  </si>
+  <si>
+    <t>degrees (deg)</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>PLAY_ERROR_SOUND</t>
+  </si>
+  <si>
+    <t>PLAY_CORRECT_SOUND</t>
+  </si>
+  <si>
+    <t>PLAY_START_SOUND</t>
+  </si>
+  <si>
+    <t>PLAY_TIMEOUT_SOUND</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Defines whether the sound of the correct answer will be played</t>
+  </si>
+  <si>
+    <t>Defines whether the sound of the incorrect answer will be played</t>
+  </si>
+  <si>
+    <t>Defines whether the sound of new trial start will be played</t>
+  </si>
+  <si>
+    <t>Defines whether the sound of timeout will be played</t>
+  </si>
+  <si>
+    <t>vestibular only, visual only, combined</t>
+  </si>
+  <si>
+    <t>combined</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>seconds (sec)</t>
+  </si>
+  <si>
+    <t>number (0 / 1)</t>
   </si>
 </sst>
 </file>
@@ -285,8 +237,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,16 +520,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="9.125" customWidth="1"/>
     <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.375" customWidth="1"/>
@@ -584,6 +537,7 @@
     <col min="7" max="7" width="9.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -591,51 +545,51 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -649,19 +603,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -675,22 +629,25 @@
       <c r="I3">
         <v>120</v>
       </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -707,57 +664,54 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -765,57 +719,57 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>315</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="H8">
-        <v>315</v>
+        <v>90</v>
       </c>
       <c r="I8">
         <v>45</v>
@@ -823,109 +777,109 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>-90</v>
+        <v>-180</v>
       </c>
       <c r="H9">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I9">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G10">
-        <v>-180</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>180</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -939,22 +893,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F13">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -968,28 +922,28 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>1.3</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -997,167 +951,155 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F15">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
       <c r="F17">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>100</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>5</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>-1</v>
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
       </c>
       <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>-1</v>
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>0</v>
+      <c r="E20" t="s">
+        <v>31</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1171,22 +1113,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>-1</v>
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="E21" t="s">
+        <v>31</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1195,184 +1137,11 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>-1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>-1</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>-1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25">
-        <v>100</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26">
-        <v>100</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>-1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
from AnyCPU to x86 (otherwise moog dll doesn't work (yet)), moog and cedrus connections
</commit_message>
<xml_diff>
--- a/Protocols/HeadingDiscrimination_test.xlsx
+++ b/Protocols/HeadingDiscrimination_test.xlsx
@@ -581,7 +581,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -656,15 +656,6 @@
       <c r="G2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -689,12 +680,6 @@
       <c r="G3" s="2">
         <v>3</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>3</v>
-      </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -809,7 +794,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>

</xml_diff>